<commit_message>
added updated images and example html downloads
</commit_message>
<xml_diff>
--- a/example_excel_files/Dan's Application Cycle Dark.xlsx
+++ b/example_excel_files/Dan's Application Cycle Dark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TooFastDan\Documents\MD_PhD Application\Cycle Analyzer\example_excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0C81F7-3264-4A2B-A1ED-DAC81D0096B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F14F5E-17FF-4D79-85C4-4C5C561EE30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{52237E55-C2FF-4619-A978-86CDA1C6CE60}"/>
   </bookViews>
@@ -152,6 +152,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -262,11 +265,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,22 +585,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1274513-DD3F-4D7E-B347-44518A37E3F5}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" style="5" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="14" style="5" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="36.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -634,238 +636,238 @@
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4">
-        <v>44383.434027777781</v>
-      </c>
-      <c r="C2" s="4">
-        <v>44388.885416666664</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="B2" s="6">
+        <v>44383</v>
+      </c>
+      <c r="C2" s="6">
+        <v>44388</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="7">
-        <v>44389.356249999997</v>
+        <v>44389</v>
       </c>
       <c r="C3" s="7">
-        <v>44396.560416666667</v>
-      </c>
-      <c r="D3" s="6"/>
+        <v>44396</v>
+      </c>
+      <c r="D3" s="7"/>
       <c r="E3" s="7">
         <v>44410.751388888886</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>44567</v>
       </c>
       <c r="G3" s="7">
         <v>44571.797222222223</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="7">
-        <v>44392.463888888888</v>
+        <v>44392</v>
       </c>
       <c r="C4" s="7">
-        <v>44401.109027777777</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+        <v>44401</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="7">
-        <v>44377.623611111114</v>
+        <v>44377</v>
       </c>
       <c r="C5" s="7">
-        <v>44383.981249999997</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+        <v>44383</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="7">
-        <v>44379.506944444445</v>
+        <v>44379</v>
       </c>
       <c r="C6" s="7">
-        <v>44385.677083333336</v>
+        <v>44385</v>
       </c>
       <c r="D6" s="7">
         <v>44476.166666666664</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="7">
-        <v>44407.84652777778</v>
+        <v>44407</v>
       </c>
       <c r="C7" s="7">
-        <v>44436.568055555559</v>
+        <v>44436</v>
       </c>
       <c r="D7" s="7">
         <v>44532.875694444447</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="7">
-        <v>44372.369444444441</v>
+        <v>44372</v>
       </c>
       <c r="C8" s="7">
-        <v>44373.215277777781</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+        <v>44373</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="7">
-        <v>44384.588194444441</v>
+        <v>44384</v>
       </c>
       <c r="C9" s="7">
         <v>44391.728472222225</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="7">
         <v>44435.523611111108</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>44476</v>
       </c>
       <c r="G9" s="7">
         <v>44568.686111111114</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="7">
-        <v>44378.465277777781</v>
+        <v>44378</v>
       </c>
       <c r="C10" s="7">
         <v>44380.9375</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="7">
         <v>44460.566666666666</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>44490</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="8">
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7">
         <v>44553</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="7">
-        <v>44386.536805555559</v>
+        <v>44386</v>
       </c>
       <c r="C11" s="7">
         <v>44394.519444444442</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="7">
         <v>44510.720833333333</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <v>44570</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="7">
-        <v>44389.25</v>
+        <v>44389</v>
       </c>
       <c r="C12" s="7">
         <v>44403.995138888888</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="7">
-        <v>44372.917361111111</v>
+        <v>44372</v>
       </c>
       <c r="C13" s="7">
         <v>44377.508333333331</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="7">
-        <v>44384.490277777775</v>
+        <v>44384</v>
       </c>
       <c r="C14" s="7">
         <v>44389.079861111109</v>
@@ -873,41 +875,41 @@
       <c r="D14" s="7">
         <v>44414.518055555556</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="7">
-        <v>44393.447222222225</v>
+        <v>44393</v>
       </c>
       <c r="C15" s="7">
         <v>44396.914583333331</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="7">
         <v>44433.750694444447</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>44461</v>
       </c>
       <c r="G15" s="7">
         <v>44491.765972222223</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="7">
-        <v>44372.6</v>
+        <v>44372</v>
       </c>
       <c r="C16" s="7">
         <v>44376.71597222222</v>
@@ -915,35 +917,35 @@
       <c r="D16" s="7">
         <v>44538.668749999997</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="7">
-        <v>44381.887499999997</v>
+        <v>44381</v>
       </c>
       <c r="C17" s="7">
         <v>44387.847222222219</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="7">
-        <v>44375.423611111109</v>
+        <v>44375</v>
       </c>
       <c r="C18" s="7">
         <v>44379.162499999999</v>
@@ -951,18 +953,18 @@
       <c r="D18" s="7">
         <v>44509.560416666667</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="7">
-        <v>44378.737500000003</v>
+        <v>44378</v>
       </c>
       <c r="C19" s="7">
         <v>44381.810416666667</v>
@@ -970,18 +972,18 @@
       <c r="D19" s="7">
         <v>44536.706250000003</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="7">
-        <v>44389.370833333334</v>
+        <v>44389</v>
       </c>
       <c r="C20" s="7">
         <v>44403.030555555553</v>
@@ -989,161 +991,161 @@
       <c r="D20" s="7">
         <v>44546.372916666667</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="7">
-        <v>44386.385416666664</v>
+        <v>44386</v>
       </c>
       <c r="C21" s="7">
         <v>44393.621527777781</v>
       </c>
-      <c r="D21" s="6"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="7">
         <v>44434.543749999997</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7">
         <v>44531</v>
       </c>
       <c r="G21" s="7">
         <v>44575.537499999999</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="7">
-        <v>44384.658333333333</v>
+        <v>44384</v>
       </c>
       <c r="C22" s="7">
         <v>44395.71597222222</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="7"/>
       <c r="E22" s="7">
         <v>44459.655555555553</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="7">
         <v>44494</v>
       </c>
       <c r="G22" s="7">
         <v>44516.5</v>
       </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="7">
-        <v>44391.208333333336</v>
+        <v>44391</v>
       </c>
       <c r="C23" s="7">
         <v>44405.402777777781</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="7">
         <v>44494.686805555553</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>44515</v>
       </c>
       <c r="G23" s="7">
         <v>44540.90902777778</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="7">
-        <v>44392.713888888888</v>
+        <v>44392</v>
       </c>
       <c r="C24" s="7">
         <v>44405.972222222219</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="7">
-        <v>44373.209027777775</v>
+        <v>44373</v>
       </c>
       <c r="C25" s="7">
         <v>44373.925694444442</v>
       </c>
-      <c r="D25" s="6"/>
+      <c r="D25" s="7"/>
       <c r="E25" s="7">
         <v>44434.718055555553</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="7">
         <v>44456</v>
       </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="7">
-        <v>44397.597916666666</v>
+        <v>44397</v>
       </c>
       <c r="C26" s="7">
         <v>44431.136805555558</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B27" s="7">
-        <v>44377.356944444444</v>
+        <v>44377</v>
       </c>
       <c r="C27" s="7">
         <v>44379.838194444441</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="8">
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7">
         <v>44573</v>
       </c>
-      <c r="I27" s="6"/>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="7">
-        <v>44378.418749999997</v>
+        <v>44378</v>
       </c>
       <c r="C28" s="7">
         <v>44382.771527777775</v>
@@ -1151,57 +1153,58 @@
       <c r="D28" s="7">
         <v>44470.67083333333</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="7">
-        <v>44383.426388888889</v>
+        <v>44383</v>
       </c>
       <c r="C29" s="7">
         <v>44388.104166666664</v>
       </c>
-      <c r="D29" s="6"/>
+      <c r="D29" s="7"/>
       <c r="E29" s="7">
         <v>44447.548611111109</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="7">
         <v>44502</v>
       </c>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="8">
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7">
         <v>44531</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B30" s="7">
-        <v>44397.61041666667</v>
+        <v>44397</v>
       </c>
       <c r="C30" s="7">
         <v>44409.80972222222</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
       <c r="G30" s="7">
         <v>44467.542361111111</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="7">
         <v>44575</v>
       </c>
-      <c r="I30" s="6"/>
+      <c r="I30" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixes and polishing
</commit_message>
<xml_diff>
--- a/example_excel_files/Dan's Application Cycle Dark.xlsx
+++ b/example_excel_files/Dan's Application Cycle Dark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TooFastDan\Documents\MD_PhD Application\Cycle Analyzer\example_excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F14F5E-17FF-4D79-85C4-4C5C561EE30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB7030E-554F-48A2-A7DD-FDE7139096AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{52237E55-C2FF-4619-A978-86CDA1C6CE60}"/>
   </bookViews>
@@ -153,7 +153,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -267,8 +267,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,7 +586,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,13 +661,13 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7">
-        <v>44410.751388888886</v>
+        <v>44410</v>
       </c>
       <c r="F3" s="7">
         <v>44567</v>
       </c>
       <c r="G3" s="7">
-        <v>44571.797222222223</v>
+        <v>44571</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -717,7 +717,7 @@
         <v>44385</v>
       </c>
       <c r="D6" s="7">
-        <v>44476.166666666664</v>
+        <v>44476</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -736,7 +736,7 @@
         <v>44436</v>
       </c>
       <c r="D7" s="7">
-        <v>44532.875694444447</v>
+        <v>44532</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -769,17 +769,17 @@
         <v>44384</v>
       </c>
       <c r="C9" s="7">
-        <v>44391.728472222225</v>
+        <v>44391</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7">
-        <v>44435.523611111108</v>
+        <v>44435</v>
       </c>
       <c r="F9" s="7">
         <v>44476</v>
       </c>
       <c r="G9" s="7">
-        <v>44568.686111111114</v>
+        <v>44568</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -792,11 +792,11 @@
         <v>44378</v>
       </c>
       <c r="C10" s="7">
-        <v>44380.9375</v>
+        <v>44380</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7">
-        <v>44460.566666666666</v>
+        <v>44460</v>
       </c>
       <c r="F10" s="7">
         <v>44490</v>
@@ -815,11 +815,11 @@
         <v>44386</v>
       </c>
       <c r="C11" s="7">
-        <v>44394.519444444442</v>
+        <v>44394</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7">
-        <v>44510.720833333333</v>
+        <v>44510</v>
       </c>
       <c r="F11" s="7">
         <v>44570</v>
@@ -836,7 +836,7 @@
         <v>44389</v>
       </c>
       <c r="C12" s="7">
-        <v>44403.995138888888</v>
+        <v>44403</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -853,7 +853,7 @@
         <v>44372</v>
       </c>
       <c r="C13" s="7">
-        <v>44377.508333333331</v>
+        <v>44377</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -870,10 +870,10 @@
         <v>44384</v>
       </c>
       <c r="C14" s="7">
-        <v>44389.079861111109</v>
+        <v>44389</v>
       </c>
       <c r="D14" s="7">
-        <v>44414.518055555556</v>
+        <v>44414</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -889,17 +889,17 @@
         <v>44393</v>
       </c>
       <c r="C15" s="7">
-        <v>44396.914583333331</v>
+        <v>44396</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7">
-        <v>44433.750694444447</v>
+        <v>44433</v>
       </c>
       <c r="F15" s="7">
         <v>44461</v>
       </c>
       <c r="G15" s="7">
-        <v>44491.765972222223</v>
+        <v>44491</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -912,10 +912,10 @@
         <v>44372</v>
       </c>
       <c r="C16" s="7">
-        <v>44376.71597222222</v>
+        <v>44376</v>
       </c>
       <c r="D16" s="7">
-        <v>44538.668749999997</v>
+        <v>44538</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -931,7 +931,7 @@
         <v>44381</v>
       </c>
       <c r="C17" s="7">
-        <v>44387.847222222219</v>
+        <v>44387</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -948,10 +948,10 @@
         <v>44375</v>
       </c>
       <c r="C18" s="7">
-        <v>44379.162499999999</v>
+        <v>44379</v>
       </c>
       <c r="D18" s="7">
-        <v>44509.560416666667</v>
+        <v>44509</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -967,10 +967,10 @@
         <v>44378</v>
       </c>
       <c r="C19" s="7">
-        <v>44381.810416666667</v>
+        <v>44381</v>
       </c>
       <c r="D19" s="7">
-        <v>44536.706250000003</v>
+        <v>44536</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -986,10 +986,10 @@
         <v>44389</v>
       </c>
       <c r="C20" s="7">
-        <v>44403.030555555553</v>
+        <v>44403</v>
       </c>
       <c r="D20" s="7">
-        <v>44546.372916666667</v>
+        <v>44546</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1005,17 +1005,17 @@
         <v>44386</v>
       </c>
       <c r="C21" s="7">
-        <v>44393.621527777781</v>
+        <v>44393</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7">
-        <v>44434.543749999997</v>
+        <v>44434</v>
       </c>
       <c r="F21" s="7">
         <v>44531</v>
       </c>
       <c r="G21" s="7">
-        <v>44575.537499999999</v>
+        <v>44575</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -1028,17 +1028,17 @@
         <v>44384</v>
       </c>
       <c r="C22" s="7">
-        <v>44395.71597222222</v>
+        <v>44395</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7">
-        <v>44459.655555555553</v>
+        <v>44459</v>
       </c>
       <c r="F22" s="7">
         <v>44494</v>
       </c>
       <c r="G22" s="7">
-        <v>44516.5</v>
+        <v>44516</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -1051,17 +1051,17 @@
         <v>44391</v>
       </c>
       <c r="C23" s="7">
-        <v>44405.402777777781</v>
+        <v>44405</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7">
-        <v>44494.686805555553</v>
+        <v>44494</v>
       </c>
       <c r="F23" s="7">
         <v>44515</v>
       </c>
       <c r="G23" s="7">
-        <v>44540.90902777778</v>
+        <v>44540</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
@@ -1074,7 +1074,7 @@
         <v>44392</v>
       </c>
       <c r="C24" s="7">
-        <v>44405.972222222219</v>
+        <v>44405</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -1091,11 +1091,11 @@
         <v>44373</v>
       </c>
       <c r="C25" s="7">
-        <v>44373.925694444442</v>
+        <v>44373</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7">
-        <v>44434.718055555553</v>
+        <v>44434</v>
       </c>
       <c r="F25" s="7">
         <v>44456</v>
@@ -1112,7 +1112,7 @@
         <v>44397</v>
       </c>
       <c r="C26" s="7">
-        <v>44431.136805555558</v>
+        <v>44431</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -1129,7 +1129,7 @@
         <v>44377</v>
       </c>
       <c r="C27" s="7">
-        <v>44379.838194444441</v>
+        <v>44379</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -1148,10 +1148,10 @@
         <v>44378</v>
       </c>
       <c r="C28" s="7">
-        <v>44382.771527777775</v>
+        <v>44382</v>
       </c>
       <c r="D28" s="7">
-        <v>44470.67083333333</v>
+        <v>44470</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -1167,11 +1167,11 @@
         <v>44383</v>
       </c>
       <c r="C29" s="7">
-        <v>44388.104166666664</v>
+        <v>44388</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7">
-        <v>44447.548611111109</v>
+        <v>44447</v>
       </c>
       <c r="F29" s="7">
         <v>44502</v>
@@ -1190,13 +1190,13 @@
         <v>44397</v>
       </c>
       <c r="C30" s="7">
-        <v>44409.80972222222</v>
+        <v>44409</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7">
-        <v>44467.542361111111</v>
+        <v>44467</v>
       </c>
       <c r="H30" s="7">
         <v>44575</v>

</xml_diff>